<commit_message>
Rename scenery to scenario
</commit_message>
<xml_diff>
--- a/cases/c0/system_c0.xlsx
+++ b/cases/c0/system_c0.xlsx
@@ -4,13 +4,13 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="2" windowWidth="18540" windowHeight="8020"/>
+    <workbookView activeTab="7" windowWidth="18540" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="options" sheetId="1" r:id="rId1"/>
     <sheet name="block_array" sheetId="2" r:id="rId2"/>
     <sheet name="stage_array" sheetId="3" r:id="rId3"/>
-    <sheet name="scenery_array" sheetId="4" r:id="rId4"/>
+    <sheet name="scenario_array" sheetId="4" r:id="rId4"/>
     <sheet name="bus_array" sheetId="5" r:id="rId5"/>
     <sheet name="generator_array" sheetId="6" r:id="rId6"/>
     <sheet name="demand_array" sheetId="7" r:id="rId7"/>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="2">"stage_array"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"scenery_array"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"scenario_array"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="4">"bus_array"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
   <si>
     <t>uid</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>d1</t>
+  </si>
+  <si>
+    <t>scenario</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -707,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -716,11 +719,9 @@
     <col min="1" max="16384" style="0" width="1.7409667968750002"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>scenery</t>
-        </is>
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" t="s">
+        <v>10</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>

</xml_diff>